<commit_message>
spostamento ottimizziazione fuori dalla generazione in loop
</commit_message>
<xml_diff>
--- a/commonFiles/dati.xlsx
+++ b/commonFiles/dati.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cross_os\sviluppo\java_projects\SuiteTurni\turniMaker\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cross_os\sviluppo\java_projects\SuiteTurni\commonFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B652948-F0BC-4191-A41B-23C74A2E75DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09058EB8-96E5-491F-B20E-9C46AC556326}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6540" yWindow="4425" windowWidth="28800" windowHeight="15555" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Persone-Indisp" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="17">
   <si>
     <t>CAR</t>
   </si>
@@ -50,28 +50,28 @@
     <t>MAR</t>
   </si>
   <si>
-    <t>MIG</t>
-  </si>
-  <si>
-    <t>FAN</t>
-  </si>
-  <si>
-    <t>LEG</t>
-  </si>
-  <si>
-    <t>SAR</t>
-  </si>
-  <si>
-    <t>BAT</t>
-  </si>
-  <si>
-    <t>BOM</t>
-  </si>
-  <si>
-    <t>AAA</t>
-  </si>
-  <si>
-    <t>ZZZ</t>
+    <t>BET</t>
+  </si>
+  <si>
+    <t>MAD</t>
+  </si>
+  <si>
+    <t>VIN</t>
+  </si>
+  <si>
+    <t>VAN</t>
+  </si>
+  <si>
+    <t>DAN</t>
+  </si>
+  <si>
+    <t>SAC</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>TOC</t>
   </si>
 </sst>
 </file>
@@ -247,10 +247,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -569,8 +569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AF13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L29" sqref="L29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -675,63 +675,156 @@
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>7</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="T10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="U10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="V10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="W10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="X10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AE10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF10" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="G11" s="14"/>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -744,8 +837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="C3:G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -755,16 +848,16 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15" t="s">
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="15"/>
+      <c r="G1" s="16"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -791,7 +884,7 @@
       <c r="A3" s="12">
         <v>44197</v>
       </c>
-      <c r="B3" s="16"/>
+      <c r="B3" s="15"/>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
       <c r="E3" s="6"/>
@@ -802,7 +895,7 @@
       <c r="A4" s="12">
         <v>44198</v>
       </c>
-      <c r="B4" s="16"/>
+      <c r="B4" s="15"/>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
       <c r="E4" s="6"/>
@@ -813,7 +906,7 @@
       <c r="A5" s="12">
         <v>44199</v>
       </c>
-      <c r="B5" s="16"/>
+      <c r="B5" s="15"/>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
       <c r="E5" s="6"/>
@@ -824,7 +917,7 @@
       <c r="A6" s="12">
         <v>44200</v>
       </c>
-      <c r="B6" s="16"/>
+      <c r="B6" s="15"/>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
       <c r="E6" s="6"/>
@@ -835,7 +928,7 @@
       <c r="A7" s="12">
         <v>44201</v>
       </c>
-      <c r="B7" s="16"/>
+      <c r="B7" s="15"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
       <c r="E7" s="6"/>
@@ -846,7 +939,7 @@
       <c r="A8" s="12">
         <v>44202</v>
       </c>
-      <c r="B8" s="16"/>
+      <c r="B8" s="15"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
       <c r="E8" s="6"/>
@@ -857,7 +950,7 @@
       <c r="A9" s="12">
         <v>44203</v>
       </c>
-      <c r="B9" s="16"/>
+      <c r="B9" s="15"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
       <c r="E9" s="6"/>
@@ -868,7 +961,7 @@
       <c r="A10" s="12">
         <v>44204</v>
       </c>
-      <c r="B10" s="16"/>
+      <c r="B10" s="15"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
       <c r="E10" s="6"/>
@@ -884,7 +977,7 @@
       <c r="A11" s="12">
         <v>44205</v>
       </c>
-      <c r="B11" s="16"/>
+      <c r="B11" s="15"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
       <c r="E11" s="6"/>
@@ -900,7 +993,7 @@
       <c r="A12" s="12">
         <v>44206</v>
       </c>
-      <c r="B12" s="16"/>
+      <c r="B12" s="15"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
       <c r="E12" s="6"/>
@@ -916,7 +1009,7 @@
       <c r="A13" s="12">
         <v>44207</v>
       </c>
-      <c r="B13" s="16"/>
+      <c r="B13" s="15"/>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
       <c r="E13" s="6"/>
@@ -932,7 +1025,7 @@
       <c r="A14" s="12">
         <v>44208</v>
       </c>
-      <c r="B14" s="16"/>
+      <c r="B14" s="15"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
       <c r="E14" s="6"/>
@@ -948,7 +1041,7 @@
       <c r="A15" s="12">
         <v>44209</v>
       </c>
-      <c r="B15" s="16"/>
+      <c r="B15" s="15"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
       <c r="E15" s="6"/>
@@ -964,7 +1057,7 @@
       <c r="A16" s="12">
         <v>44210</v>
       </c>
-      <c r="B16" s="16"/>
+      <c r="B16" s="15"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
       <c r="E16" s="6"/>
@@ -980,7 +1073,7 @@
       <c r="A17" s="12">
         <v>44211</v>
       </c>
-      <c r="B17" s="16"/>
+      <c r="B17" s="15"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
       <c r="E17" s="6"/>
@@ -996,7 +1089,7 @@
       <c r="A18" s="12">
         <v>44212</v>
       </c>
-      <c r="B18" s="16"/>
+      <c r="B18" s="15"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
       <c r="E18" s="6"/>
@@ -1012,7 +1105,7 @@
       <c r="A19" s="12">
         <v>44213</v>
       </c>
-      <c r="B19" s="16"/>
+      <c r="B19" s="15"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
       <c r="E19" s="6"/>
@@ -1028,7 +1121,7 @@
       <c r="A20" s="12">
         <v>44214</v>
       </c>
-      <c r="B20" s="16"/>
+      <c r="B20" s="15"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
       <c r="E20" s="6"/>
@@ -1044,7 +1137,7 @@
       <c r="A21" s="12">
         <v>44215</v>
       </c>
-      <c r="B21" s="16"/>
+      <c r="B21" s="15"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
       <c r="E21" s="6"/>
@@ -1055,7 +1148,7 @@
       <c r="A22" s="12">
         <v>44216</v>
       </c>
-      <c r="B22" s="16"/>
+      <c r="B22" s="15"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
       <c r="E22" s="6"/>
@@ -1066,7 +1159,7 @@
       <c r="A23" s="12">
         <v>44217</v>
       </c>
-      <c r="B23" s="16"/>
+      <c r="B23" s="15"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
       <c r="E23" s="6"/>
@@ -1077,7 +1170,7 @@
       <c r="A24" s="12">
         <v>44218</v>
       </c>
-      <c r="B24" s="16"/>
+      <c r="B24" s="15"/>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
       <c r="E24" s="6"/>
@@ -1088,7 +1181,7 @@
       <c r="A25" s="12">
         <v>44219</v>
       </c>
-      <c r="B25" s="16"/>
+      <c r="B25" s="15"/>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
       <c r="E25" s="6"/>
@@ -1099,7 +1192,7 @@
       <c r="A26" s="12">
         <v>44220</v>
       </c>
-      <c r="B26" s="16"/>
+      <c r="B26" s="15"/>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
       <c r="E26" s="6"/>
@@ -1110,7 +1203,7 @@
       <c r="A27" s="12">
         <v>44221</v>
       </c>
-      <c r="B27" s="16"/>
+      <c r="B27" s="15"/>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
       <c r="E27" s="6"/>
@@ -1121,7 +1214,7 @@
       <c r="A28" s="12">
         <v>44222</v>
       </c>
-      <c r="B28" s="16"/>
+      <c r="B28" s="15"/>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
       <c r="E28" s="6"/>
@@ -1132,7 +1225,7 @@
       <c r="A29" s="12">
         <v>44223</v>
       </c>
-      <c r="B29" s="16"/>
+      <c r="B29" s="15"/>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
       <c r="E29" s="6"/>
@@ -1143,7 +1236,7 @@
       <c r="A30" s="12">
         <v>44224</v>
       </c>
-      <c r="B30" s="16"/>
+      <c r="B30" s="15"/>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
       <c r="E30" s="6"/>
@@ -1154,7 +1247,7 @@
       <c r="A31" s="12">
         <v>44225</v>
       </c>
-      <c r="B31" s="16"/>
+      <c r="B31" s="15"/>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
       <c r="E31" s="6"/>
@@ -1165,7 +1258,7 @@
       <c r="A32" s="12">
         <v>44226</v>
       </c>
-      <c r="B32" s="16"/>
+      <c r="B32" s="15"/>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
       <c r="E32" s="6"/>

</xml_diff>

<commit_message>
versione funzionante e testata
</commit_message>
<xml_diff>
--- a/commonFiles/dati.xlsx
+++ b/commonFiles/dati.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cross_os\sviluppo\java_projects\SuiteTurni\commonFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50174805-A361-41C7-89CE-BAA7FF7B8EC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6795FB31-AEE0-4026-8695-FB1BBB3F3305}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="1440" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Persone-Indisp" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="17">
   <si>
     <t>CAR</t>
   </si>
@@ -71,13 +71,7 @@
     <t>N</t>
   </si>
   <si>
-    <t>POL</t>
-  </si>
-  <si>
     <t>GN</t>
-  </si>
-  <si>
-    <t>VAR</t>
   </si>
 </sst>
 </file>
@@ -241,9 +235,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -260,6 +251,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -578,8 +572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AF12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AC6" sqref="AC6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -690,16 +684,16 @@
         <v>15</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.25">
@@ -715,10 +709,10 @@
         <v>15</v>
       </c>
       <c r="X4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Y4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.25">
@@ -734,7 +728,7 @@
         <v>15</v>
       </c>
       <c r="AC6" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.25">
@@ -750,10 +744,10 @@
         <v>15</v>
       </c>
       <c r="X8" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Y8" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.25">
@@ -764,10 +758,10 @@
         <v>15</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.25">
@@ -882,10 +876,10 @@
         <v>15</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -898,8 +892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -909,16 +903,16 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9" t="s">
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="9"/>
+      <c r="G1" s="15"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -945,18 +939,18 @@
       <c r="A3" s="6">
         <v>44197</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10" t="s">
+      <c r="B3" s="9"/>
+      <c r="C3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="11"/>
-      <c r="F3" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="11" t="s">
+      <c r="E3" s="10"/>
+      <c r="F3" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="10" t="s">
         <v>10</v>
       </c>
     </row>
@@ -964,18 +958,18 @@
       <c r="A4" s="6">
         <v>44198</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10" t="s">
+      <c r="B4" s="9"/>
+      <c r="C4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="11"/>
-      <c r="F4" s="12" t="s">
+      <c r="D4" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="10"/>
+      <c r="F4" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="10" t="s">
         <v>5</v>
       </c>
     </row>
@@ -983,85 +977,85 @@
       <c r="A5" s="6">
         <v>44199</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="10" t="s">
+      <c r="B5" s="9"/>
+      <c r="C5" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="11"/>
-      <c r="F5" s="12" t="s">
+      <c r="E5" s="10"/>
+      <c r="F5" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="11" t="s">
-        <v>8</v>
+      <c r="G5" s="10" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>44200</v>
       </c>
-      <c r="B6" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="11"/>
+      <c r="B6" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="10"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>44201</v>
       </c>
-      <c r="B7" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="11"/>
+      <c r="B7" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="10"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>44202</v>
       </c>
-      <c r="B8" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="11"/>
+      <c r="B8" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="10"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>44203</v>
       </c>
-      <c r="B9" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="11"/>
+      <c r="B9" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="10"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>44204</v>
       </c>
-      <c r="B10" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="11"/>
+      <c r="B10" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="10"/>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
@@ -1072,12 +1066,12 @@
       <c r="A11" s="6">
         <v>44205</v>
       </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="11"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="10"/>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
@@ -1088,12 +1082,12 @@
       <c r="A12" s="6">
         <v>44206</v>
       </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="11"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="10"/>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
@@ -1104,14 +1098,14 @@
       <c r="A13" s="6">
         <v>44207</v>
       </c>
-      <c r="B13" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="11"/>
+      <c r="B13" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="10"/>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
@@ -1122,14 +1116,14 @@
       <c r="A14" s="6">
         <v>44208</v>
       </c>
-      <c r="B14" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="11"/>
+      <c r="B14" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="10"/>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
@@ -1140,14 +1134,14 @@
       <c r="A15" s="6">
         <v>44209</v>
       </c>
-      <c r="B15" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="11"/>
+      <c r="B15" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="10"/>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
@@ -1158,14 +1152,14 @@
       <c r="A16" s="6">
         <v>44210</v>
       </c>
-      <c r="B16" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="11"/>
+      <c r="B16" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="10"/>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
@@ -1176,14 +1170,14 @@
       <c r="A17" s="6">
         <v>44211</v>
       </c>
-      <c r="B17" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="11"/>
+      <c r="B17" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="10"/>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
@@ -1194,12 +1188,12 @@
       <c r="A18" s="6">
         <v>44212</v>
       </c>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="11"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="10"/>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
@@ -1210,12 +1204,12 @@
       <c r="A19" s="6">
         <v>44213</v>
       </c>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="11"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="10"/>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
@@ -1226,14 +1220,14 @@
       <c r="A20" s="6">
         <v>44214</v>
       </c>
-      <c r="B20" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="11"/>
+      <c r="B20" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="10"/>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
@@ -1244,162 +1238,162 @@
       <c r="A21" s="6">
         <v>44215</v>
       </c>
-      <c r="B21" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="11"/>
+      <c r="B21" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="10"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <v>44216</v>
       </c>
-      <c r="B22" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="11"/>
+      <c r="B22" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="10"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>44217</v>
       </c>
-      <c r="B23" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="11"/>
+      <c r="B23" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="10"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <v>44218</v>
       </c>
-      <c r="B24" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="11"/>
+      <c r="B24" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="10"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>44219</v>
       </c>
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="11"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="10"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <v>44220</v>
       </c>
-      <c r="B26" s="10"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="11"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="10"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
         <v>44221</v>
       </c>
-      <c r="B27" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="11"/>
+      <c r="B27" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="10"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
         <v>44222</v>
       </c>
-      <c r="B28" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="11"/>
+      <c r="B28" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="10"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
         <v>44223</v>
       </c>
-      <c r="B29" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="12"/>
-      <c r="G29" s="11"/>
+      <c r="B29" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="10"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
         <v>44224</v>
       </c>
-      <c r="B30" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="12"/>
-      <c r="G30" s="11"/>
+      <c r="B30" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="10"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
         <v>44225</v>
       </c>
-      <c r="B31" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="11"/>
-      <c r="F31" s="12"/>
-      <c r="G31" s="11"/>
+      <c r="B31" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="10"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="6">
         <v>44226</v>
       </c>
-      <c r="B32" s="10"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="11"/>
-      <c r="F32" s="12"/>
-      <c r="G32" s="11"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="10"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="7">
         <v>44227</v>
       </c>
-      <c r="B33" s="13"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="15"/>
-      <c r="G33" s="14"/>
+      <c r="B33" s="12"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="14"/>
+      <c r="G33" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
fix varie su generazioni
</commit_message>
<xml_diff>
--- a/commonFiles/dati.xlsx
+++ b/commonFiles/dati.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cross_os\sviluppo\java_projects\SuiteTurni\commonFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6795FB31-AEE0-4026-8695-FB1BBB3F3305}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{689FD4CC-0E8C-4D2D-A056-46997E3CBB89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1440" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Persone-Indisp" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="17">
   <si>
     <t>CAR</t>
   </si>
@@ -113,7 +113,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -155,30 +155,8 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -213,7 +191,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -226,10 +204,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -242,12 +220,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -893,7 +865,7 @@
   <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -903,16 +875,16 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15" t="s">
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="15"/>
+      <c r="G1" s="13"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -1054,8 +1026,12 @@
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
       <c r="E10" s="10"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="10"/>
+      <c r="F10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
@@ -1067,11 +1043,18 @@
         <v>44205</v>
       </c>
       <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="10"/>
+      <c r="C11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
@@ -1083,11 +1066,18 @@
         <v>44206</v>
       </c>
       <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="10"/>
+      <c r="C12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
@@ -1176,8 +1166,12 @@
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
       <c r="E17" s="10"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="10"/>
+      <c r="F17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
@@ -1189,11 +1183,18 @@
         <v>44212</v>
       </c>
       <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="10"/>
+      <c r="C18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
@@ -1205,11 +1206,18 @@
         <v>44213</v>
       </c>
       <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="10"/>
+      <c r="C19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
@@ -1283,30 +1291,48 @@
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
       <c r="E24" s="10"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="10"/>
+      <c r="F24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>44219</v>
       </c>
       <c r="B25" s="9"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="10"/>
+      <c r="C25" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <v>44220</v>
       </c>
       <c r="B26" s="9"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="10"/>
+      <c r="C26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
@@ -1370,30 +1396,46 @@
       <c r="C31" s="9"/>
       <c r="D31" s="9"/>
       <c r="E31" s="10"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="10"/>
+      <c r="F31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="6">
         <v>44226</v>
       </c>
       <c r="B32" s="9"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="11"/>
-      <c r="G32" s="10"/>
+      <c r="C32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="7">
         <v>44227</v>
       </c>
       <c r="B33" s="12"/>
-      <c r="C33" s="12"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="14"/>
-      <c r="G33" s="13"/>
+      <c r="C33" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G33" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
vecchie commit rimaste li da chissà quanto
</commit_message>
<xml_diff>
--- a/commonFiles/dati.xlsx
+++ b/commonFiles/dati.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cross_os\sviluppo\java_projects\SuiteTurni\commonFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{689FD4CC-0E8C-4D2D-A056-46997E3CBB89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6795FB31-AEE0-4026-8695-FB1BBB3F3305}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="1440" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Persone-Indisp" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="17">
   <si>
     <t>CAR</t>
   </si>
@@ -113,7 +113,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -155,8 +155,30 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -191,7 +213,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -204,10 +226,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -220,6 +242,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -865,7 +893,7 @@
   <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -875,16 +903,16 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13" t="s">
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="13"/>
+      <c r="G1" s="15"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -1026,12 +1054,8 @@
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
       <c r="E10" s="10"/>
-      <c r="F10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="F10" s="11"/>
+      <c r="G10" s="10"/>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
@@ -1043,18 +1067,11 @@
         <v>44205</v>
       </c>
       <c r="B11" s="9"/>
-      <c r="C11" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="10"/>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
@@ -1066,18 +1083,11 @@
         <v>44206</v>
       </c>
       <c r="B12" s="9"/>
-      <c r="C12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="10"/>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
@@ -1166,12 +1176,8 @@
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
       <c r="E17" s="10"/>
-      <c r="F17" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="F17" s="11"/>
+      <c r="G17" s="10"/>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
@@ -1183,18 +1189,11 @@
         <v>44212</v>
       </c>
       <c r="B18" s="9"/>
-      <c r="C18" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="10"/>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
@@ -1206,18 +1205,11 @@
         <v>44213</v>
       </c>
       <c r="B19" s="9"/>
-      <c r="C19" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="10"/>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
@@ -1291,48 +1283,30 @@
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
       <c r="E24" s="10"/>
-      <c r="F24" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F24" s="11"/>
+      <c r="G24" s="10"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>44219</v>
       </c>
       <c r="B25" s="9"/>
-      <c r="C25" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="10"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <v>44220</v>
       </c>
       <c r="B26" s="9"/>
-      <c r="C26" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="10"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
@@ -1396,46 +1370,30 @@
       <c r="C31" s="9"/>
       <c r="D31" s="9"/>
       <c r="E31" s="10"/>
-      <c r="F31" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="F31" s="11"/>
+      <c r="G31" s="10"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="6">
         <v>44226</v>
       </c>
       <c r="B32" s="9"/>
-      <c r="C32" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="10"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="7">
         <v>44227</v>
       </c>
       <c r="B33" s="12"/>
-      <c r="C33" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G33" s="8"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="14"/>
+      <c r="G33" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>